<commit_message>
- bulk and rttask period run with sleep - TESTED for bulk and rttask wakeup
</commit_message>
<xml_diff>
--- a/Doc/docs.xlsx
+++ b/Doc/docs.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="01_Generic_stuff" sheetId="1" r:id="rId1"/>
     <sheet name="02_HW_Components" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Power source" sheetId="3" r:id="rId3"/>
+    <sheet name="ExtFlash" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="111">
   <si>
     <t>microcontroller:</t>
   </si>
@@ -178,13 +179,184 @@
   </si>
   <si>
     <t>0Ohm resistor strap to link Vbatt to Vcc (if direct connection to battery)</t>
+  </si>
+  <si>
+    <t>to buy</t>
+  </si>
+  <si>
+    <t>small smd shotky diodes  (100mA)</t>
+  </si>
+  <si>
+    <t>supercap</t>
+  </si>
+  <si>
+    <t>Calculations for XC9264B75DER-G:</t>
+  </si>
+  <si>
+    <t>V.in</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>Cfb</t>
+  </si>
+  <si>
+    <t>nF</t>
+  </si>
+  <si>
+    <t>V.out</t>
+  </si>
+  <si>
+    <t>Rfb2</t>
+  </si>
+  <si>
+    <t>kOhm</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>uH</t>
+  </si>
+  <si>
+    <t>fzfb</t>
+  </si>
+  <si>
+    <t>Hz</t>
+  </si>
+  <si>
+    <t>Rfb1</t>
+  </si>
+  <si>
+    <t>Vfb</t>
+  </si>
+  <si>
+    <t>Vout</t>
+  </si>
+  <si>
+    <t xml:space="preserve">write power req. </t>
+  </si>
+  <si>
+    <t>50mA</t>
+  </si>
+  <si>
+    <t>Von min</t>
+  </si>
+  <si>
+    <t>2.7V</t>
+  </si>
+  <si>
+    <t>Vcut</t>
+  </si>
+  <si>
+    <t>2.4V</t>
+  </si>
+  <si>
+    <t>read power req.</t>
+  </si>
+  <si>
+    <t>15mA</t>
+  </si>
+  <si>
+    <t>with 20MHz clock</t>
+  </si>
+  <si>
+    <t>stdby</t>
+  </si>
+  <si>
+    <t>30uA</t>
+  </si>
+  <si>
+    <t>T reset pulse</t>
+  </si>
+  <si>
+    <t>200ns</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>T reset procedure</t>
+  </si>
+  <si>
+    <t>100us</t>
+  </si>
+  <si>
+    <t>T page prog 256</t>
+  </si>
+  <si>
+    <t xml:space="preserve">450us </t>
+  </si>
+  <si>
+    <t>1350us</t>
+  </si>
+  <si>
+    <t>max:</t>
+  </si>
+  <si>
+    <t>typ:</t>
+  </si>
+  <si>
+    <t>T byte prog 1st</t>
+  </si>
+  <si>
+    <t>75us</t>
+  </si>
+  <si>
+    <t>90us</t>
+  </si>
+  <si>
+    <t>T byte prog next</t>
+  </si>
+  <si>
+    <t>10us</t>
+  </si>
+  <si>
+    <t>30us</t>
+  </si>
+  <si>
+    <t>T err sector 4k</t>
+  </si>
+  <si>
+    <t>65ms</t>
+  </si>
+  <si>
+    <t>320ms</t>
+  </si>
+  <si>
+    <t>T err 1/2bk 32kB</t>
+  </si>
+  <si>
+    <t>300ms</t>
+  </si>
+  <si>
+    <t>600ms</t>
+  </si>
+  <si>
+    <t>T err bk 64kB</t>
+  </si>
+  <si>
+    <t>450ms</t>
+  </si>
+  <si>
+    <t>1150ms</t>
+  </si>
+  <si>
+    <t>T err all</t>
+  </si>
+  <si>
+    <t>55s</t>
+  </si>
+  <si>
+    <t>150s</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -202,6 +374,22 @@
     <font>
       <sz val="12"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="4" tint="-0.499984740745262"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -239,7 +427,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -253,6 +441,8 @@
     <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -556,7 +746,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
@@ -672,10 +862,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:J6"/>
+  <dimension ref="A2:J17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -836,6 +1026,19 @@
         <v>28</v>
       </c>
     </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>54</v>
+      </c>
+      <c r="B16" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>56</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -843,12 +1046,307 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A3:G16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E5" t="s">
+        <v>60</v>
+      </c>
+      <c r="F5" s="5">
+        <f>1/(2*PI() * C8 * C9* 1000) * 1000000000</f>
+        <v>0.31830988618379069</v>
+      </c>
+      <c r="G5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6">
+        <v>3.3</v>
+      </c>
+      <c r="D6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E6" t="s">
+        <v>63</v>
+      </c>
+      <c r="F6" s="5">
+        <f>(0.75*C9)/(C6-0.75)</f>
+        <v>29.411764705882355</v>
+      </c>
+      <c r="G6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8">
+        <v>5000</v>
+      </c>
+      <c r="D8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C9">
+        <v>100</v>
+      </c>
+      <c r="D9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>70</v>
+      </c>
+      <c r="C13">
+        <v>0.75</v>
+      </c>
+      <c r="D13">
+        <v>0.73899999999999999</v>
+      </c>
+      <c r="E13">
+        <v>0.76100000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>69</v>
+      </c>
+      <c r="C14">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>71</v>
+      </c>
+      <c r="C16" s="6">
+        <f>C13*($C$14+$C$15)/$C$15</f>
+        <v>3.0227272727272729</v>
+      </c>
+      <c r="D16" s="6">
+        <f>D13*($C$14+$C$15)/$C$15</f>
+        <v>2.9783939393939391</v>
+      </c>
+      <c r="E16" s="6">
+        <f>E13*($C$14+$C$15)/$C$15</f>
+        <v>3.0670606060606063</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:E18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D9" t="s">
+        <v>84</v>
+      </c>
+      <c r="E9" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>86</v>
+      </c>
+      <c r="D10" t="s">
+        <v>87</v>
+      </c>
+      <c r="E10" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>92</v>
+      </c>
+      <c r="E11" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>88</v>
+      </c>
+      <c r="D12" t="s">
+        <v>89</v>
+      </c>
+      <c r="E12" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>93</v>
+      </c>
+      <c r="D13" t="s">
+        <v>94</v>
+      </c>
+      <c r="E13" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>96</v>
+      </c>
+      <c r="D14" t="s">
+        <v>97</v>
+      </c>
+      <c r="E14" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>99</v>
+      </c>
+      <c r="D15" t="s">
+        <v>100</v>
+      </c>
+      <c r="E15" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>102</v>
+      </c>
+      <c r="D16" t="s">
+        <v>103</v>
+      </c>
+      <c r="E16" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>105</v>
+      </c>
+      <c r="D17" t="s">
+        <v>106</v>
+      </c>
+      <c r="E17" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>108</v>
+      </c>
+      <c r="D18" t="s">
+        <v>109</v>
+      </c>
+      <c r="E18" t="s">
+        <v>110</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added working hours i2c
</commit_message>
<xml_diff>
--- a/Doc/docs.xlsx
+++ b/Doc/docs.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="162">
   <si>
     <t>microcontroller:</t>
   </si>
@@ -495,6 +495,15 @@
   </si>
   <si>
     <t>interface creation for i2c and Barometer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">i2c </t>
+  </si>
+  <si>
+    <t>driver first exp.</t>
+  </si>
+  <si>
+    <t>write operation</t>
   </si>
 </sst>
 </file>
@@ -1221,7 +1230,7 @@
   <dimension ref="B2:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1231,7 +1240,7 @@
     <col min="4" max="4" width="9.140625" style="1"/>
     <col min="7" max="7" width="17.140625" customWidth="1"/>
     <col min="8" max="8" width="15.85546875" customWidth="1"/>
-    <col min="9" max="9" width="19.42578125" style="7" customWidth="1"/>
+    <col min="9" max="9" width="22.140625" style="7" customWidth="1"/>
     <col min="10" max="10" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -1361,12 +1370,27 @@
       <c r="D13" s="1">
         <v>1</v>
       </c>
+      <c r="H13" t="s">
+        <v>159</v>
+      </c>
+      <c r="I13" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="J13" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
         <v>155</v>
       </c>
       <c r="D14" s="1">
+        <v>2</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="J14" s="1">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
- finished first crude version of the i2c driver - basic test are done
</commit_message>
<xml_diff>
--- a/Doc/docs.xlsx
+++ b/Doc/docs.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="164">
   <si>
     <t>microcontroller:</t>
   </si>
@@ -504,6 +504,12 @@
   </si>
   <si>
     <t>write operation</t>
+  </si>
+  <si>
+    <t>finalizing driver and losing everything</t>
+  </si>
+  <si>
+    <t>remaking the lost stuff from head + testing</t>
   </si>
 </sst>
 </file>
@@ -1230,7 +1236,7 @@
   <dimension ref="B2:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1240,7 +1246,7 @@
     <col min="4" max="4" width="9.140625" style="1"/>
     <col min="7" max="7" width="17.140625" customWidth="1"/>
     <col min="8" max="8" width="15.85546875" customWidth="1"/>
-    <col min="9" max="9" width="22.140625" style="7" customWidth="1"/>
+    <col min="9" max="9" width="40.28515625" style="7" customWidth="1"/>
     <col min="10" max="10" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -1400,6 +1406,20 @@
       </c>
       <c r="D15" s="1">
         <v>4</v>
+      </c>
+      <c r="I15" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="J15" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I16" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="J16" s="1">
+        <v>0.5</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
@@ -2070,8 +2090,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
- fixed nxpbaro sensor read issues - conversions are still bad - upcoming fix
</commit_message>
<xml_diff>
--- a/Doc/docs.xlsx
+++ b/Doc/docs.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="171">
   <si>
     <t>microcontroller:</t>
   </si>
@@ -519,6 +519,18 @@
   </si>
   <si>
     <t xml:space="preserve">further impl. + tests, fixes </t>
+  </si>
+  <si>
+    <t>Baro Sensor</t>
+  </si>
+  <si>
+    <t>implementation</t>
+  </si>
+  <si>
+    <t>implementation finalize - testing - error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">debugging </t>
   </si>
 </sst>
 </file>
@@ -1245,7 +1257,7 @@
   <dimension ref="B2:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1466,6 +1478,15 @@
       <c r="D19" s="1">
         <v>0.5</v>
       </c>
+      <c r="H19" t="s">
+        <v>167</v>
+      </c>
+      <c r="I19" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="J19" s="1">
+        <v>4</v>
+      </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C20" s="11" t="s">
@@ -1474,6 +1495,12 @@
       <c r="D20" s="12">
         <v>0.5</v>
       </c>
+      <c r="I20" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="J20" s="1">
+        <v>8</v>
+      </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C21" s="11" t="s">
@@ -1481,6 +1508,12 @@
       </c>
       <c r="D21" s="12">
         <v>0.75</v>
+      </c>
+      <c r="I21" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="J21" s="1">
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">

</xml_diff>